<commit_message>
cierre de 10 de Nov 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/CREDITOS  4 CARNES   Z A V A L E T A    Octubre    2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/CREDITOS  4 CARNES   Z A V A L E T A    Octubre    2021.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>REMISION</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>falta la rosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1104,8 @@
   </sheetPr>
   <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1204,7 @@
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="64" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" s="20">
         <v>0</v>
@@ -2066,83 +2069,113 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="12">
+        <v>44501</v>
+      </c>
       <c r="B40" s="13">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C40" s="24"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20"/>
+      <c r="D40" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="20">
+        <v>259</v>
+      </c>
       <c r="F40" s="21"/>
       <c r="G40" s="22"/>
       <c r="H40" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="12">
+        <v>44502</v>
+      </c>
       <c r="B41" s="13">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C41" s="24"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
+      <c r="D41" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="20">
+        <v>8605</v>
+      </c>
       <c r="F41" s="21"/>
       <c r="G41" s="22"/>
       <c r="H41" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8605</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="12">
+        <v>44503</v>
+      </c>
       <c r="B42" s="13">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C42" s="24"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
+      <c r="D42" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="20">
+        <v>235</v>
+      </c>
       <c r="F42" s="21"/>
       <c r="G42" s="22"/>
       <c r="H42" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+      <c r="A43" s="12">
+        <v>44505</v>
+      </c>
       <c r="B43" s="13">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C43" s="24"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
+      <c r="D43" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="20">
+        <v>1618</v>
+      </c>
       <c r="F43" s="21"/>
       <c r="G43" s="22"/>
       <c r="H43" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+      <c r="A44" s="12">
+        <v>44505</v>
+      </c>
       <c r="B44" s="13">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C44" s="24"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="20"/>
+      <c r="D44" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="20">
+        <v>784</v>
+      </c>
       <c r="F44" s="21"/>
       <c r="G44" s="22"/>
       <c r="H44" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>784</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3294,7 +3327,7 @@
       <c r="D117" s="2"/>
       <c r="E117" s="39">
         <f>SUM(E4:E116)</f>
-        <v>1106633</v>
+        <v>1118134</v>
       </c>
       <c r="F117" s="39"/>
       <c r="G117" s="39">
@@ -3303,7 +3336,7 @@
       </c>
       <c r="H117" s="40">
         <f>SUM(H4:H116)</f>
-        <v>91095</v>
+        <v>102596</v>
       </c>
       <c r="I117" s="2"/>
     </row>
@@ -3347,7 +3380,7 @@
       <c r="D121" s="2"/>
       <c r="E121" s="78">
         <f>E117-G117</f>
-        <v>91095</v>
+        <v>102596</v>
       </c>
       <c r="F121" s="79"/>
       <c r="G121" s="80"/>

</xml_diff>